<commit_message>
Proyecto finalizado versión 1.0
</commit_message>
<xml_diff>
--- a/dist/prointe-front/assets/bd/servicios.xlsx
+++ b/dist/prointe-front/assets/bd/servicios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\Proyectos-Recap\plantillas\plantilla1\prointeFront\src\assets\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1A8B43-E8D7-40D0-8D8B-79CB0B0C758E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FF60FB-02DB-4932-A09F-EE9323985741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t xml:space="preserve">id </t>
   </si>
@@ -81,7 +81,22 @@
     <t>imagen</t>
   </si>
   <si>
-    <t>/assets/img/productos/extintores5-10-20.webp</t>
+    <t>/assets/img/productos/extintores/extintor-5-lbs-co2.png</t>
+  </si>
+  <si>
+    <t>/assets/img/productos/extintores/Extintor-10-lbs-pqs.png</t>
+  </si>
+  <si>
+    <t>/assets/img/productos/extintores/10-lbs-co2-1.png</t>
+  </si>
+  <si>
+    <t>/assets/img/productos/extintores/EXTINTOR-5-LBS-PQS.png</t>
+  </si>
+  <si>
+    <t>/assets/img/productos/extintores/EXTINTOR-20-LBS-PQS.png</t>
+  </si>
+  <si>
+    <t>/assets/img/productos/extintores/1-11.png</t>
   </si>
 </sst>
 </file>
@@ -430,7 +445,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,7 +503,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -505,7 +520,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -522,7 +537,7 @@
         <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -539,7 +554,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -556,7 +571,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>